<commit_message>
performs multiple runs, saves separate files
</commit_message>
<xml_diff>
--- a/results/approved_voters=10_projects=6.xlsx
+++ b/results/approved_voters=10_projects=6.xlsx
@@ -476,16 +476,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -526,16 +526,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -563,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -657,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -751,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -801,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>

</xml_diff>